<commit_message>
Updated index.js and modified excel
</commit_message>
<xml_diff>
--- a/configs/DealerConfiguration.xlsx
+++ b/configs/DealerConfiguration.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -102,19 +102,19 @@
     <t>Ford The</t>
   </si>
   <si>
-    <t xml:space="preserve">   Ford With Spaces    </t>
-  </si>
-  <si>
     <t>5,7,8,9</t>
   </si>
   <si>
     <t>3,4,5,6</t>
+  </si>
+  <si>
+    <t>Ford With Spaces</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
@@ -180,6 +180,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -227,7 +230,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,7 +265,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -474,7 +477,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +767,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
@@ -790,10 +793,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>11</v>

</xml_diff>